<commit_message>
clean up input a bit
</commit_message>
<xml_diff>
--- a/my_code/my_model_2/input/MH_trans.xlsx
+++ b/my_code/my_model_2/input/MH_trans.xlsx
@@ -1,26 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\My Drive\PhD\PhD Year 3\3rd Year Paper\Model\My Code\MH_Model\my_code\my_model_2\input\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197FD0C1-D375-4607-A378-20802D0AD241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Figure1_MH" sheetId="1" r:id="rId1"/>
+    <sheet name="Figure1_MH" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="7">
+  <si>
+    <t>Bad MH Type : % transition from bad mental health</t>
+  </si>
   <si>
     <t>age</t>
   </si>
@@ -29,9 +25,6 @@
   </si>
   <si>
     <t>to good</t>
-  </si>
-  <si>
-    <t>Bad MH Type : % transition from bad mental health</t>
   </si>
   <si>
     <t>Good MH Type : % transition from bad mental health</t>
@@ -46,8 +39,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -79,347 +72,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="0E2841"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="156082"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="E97132"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="196B24"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="A02B93"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="4EA72E"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="467886"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="96607D"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V53"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -431,1983 +94,1982 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
+      <c r="O2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" t="s">
         <v>2</v>
       </c>
-      <c r="N2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="T2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" t="s">
         <v>2</v>
       </c>
-      <c r="P2" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U2" t="s">
-        <v>2</v>
-      </c>
-      <c r="V2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3">
       <c r="A3">
         <v>25</v>
       </c>
       <c r="B3">
-        <v>0.76778898471595658</v>
+        <v>0.87653022511838263</v>
       </c>
       <c r="C3">
-        <v>0.23221101528404345</v>
+        <v>0.12346977488161737</v>
       </c>
       <c r="H3">
         <v>25</v>
       </c>
       <c r="I3">
-        <v>0.59640338456004538</v>
+        <v>0.39822453931279728</v>
       </c>
       <c r="J3">
-        <v>0.40359661543995456</v>
+        <v>0.60177546068720267</v>
       </c>
       <c r="N3">
         <v>25</v>
       </c>
       <c r="O3">
-        <v>0.59640338456004538</v>
+        <v>0.29423497731104881</v>
       </c>
       <c r="P3">
-        <v>0.40359661543995456</v>
+        <v>0.70576502268895114</v>
       </c>
       <c r="T3">
         <v>25</v>
       </c>
       <c r="U3">
-        <v>0.70292646764843347</v>
+        <v>0.78162556294991981</v>
       </c>
       <c r="V3">
-        <v>0.29707353235156658</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.21837443705008014</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4">
         <v>26</v>
       </c>
       <c r="B4">
-        <v>0.76087199158706087</v>
+        <v>0.87395627205409987</v>
       </c>
       <c r="C4">
-        <v>0.23912800841293905</v>
+        <v>0.1260437279459001</v>
       </c>
       <c r="H4">
         <v>26</v>
       </c>
       <c r="I4">
-        <v>0.56363151124710353</v>
+        <v>0.37658319050759193</v>
       </c>
       <c r="J4">
-        <v>0.43636848875289652</v>
+        <v>0.62341680949240807</v>
       </c>
       <c r="N4">
         <v>26</v>
       </c>
       <c r="O4">
-        <v>0.56363151124710353</v>
+        <v>0.29252559130432365</v>
       </c>
       <c r="P4">
-        <v>0.43636848875289652</v>
+        <v>0.70747440869567635</v>
       </c>
       <c r="T4">
         <v>26</v>
       </c>
       <c r="U4">
-        <v>0.69663867063322071</v>
+        <v>0.76819313097250685</v>
       </c>
       <c r="V4">
-        <v>0.30336132936677929</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.23180686902749317</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5">
         <v>27</v>
       </c>
       <c r="B5">
-        <v>0.75105442289042312</v>
+        <v>0.82499847165683271</v>
       </c>
       <c r="C5">
-        <v>0.24894557710957699</v>
+        <v>0.17500152834316729</v>
       </c>
       <c r="H5">
         <v>27</v>
       </c>
       <c r="I5">
-        <v>0.4481319815049839</v>
+        <v>0.34404688368294079</v>
       </c>
       <c r="J5">
-        <v>0.5518680184950161</v>
+        <v>0.65595311631705921</v>
       </c>
       <c r="N5">
         <v>27</v>
       </c>
       <c r="O5">
-        <v>0.4481319815049839</v>
+        <v>0.25504018553691471</v>
       </c>
       <c r="P5">
-        <v>0.5518680184950161</v>
+        <v>0.74495981446308523</v>
       </c>
       <c r="T5">
         <v>27</v>
       </c>
       <c r="U5">
-        <v>0.71162270570056818</v>
+        <v>0.77949984955494234</v>
       </c>
       <c r="V5">
-        <v>0.28837729429943171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.22050015044505775</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6">
         <v>28</v>
       </c>
       <c r="B6">
-        <v>0.74645742019740002</v>
+        <v>0.8575775352415177</v>
       </c>
       <c r="C6">
-        <v>0.25354257980259992</v>
+        <v>0.14242246475848225</v>
       </c>
       <c r="H6">
         <v>28</v>
       </c>
       <c r="I6">
-        <v>0.6155241036870448</v>
+        <v>0.43625590660398045</v>
       </c>
       <c r="J6">
-        <v>0.38447589631295526</v>
+        <v>0.56374409339601961</v>
       </c>
       <c r="N6">
         <v>28</v>
       </c>
       <c r="O6">
-        <v>0.6155241036870448</v>
+        <v>0.18852078063785588</v>
       </c>
       <c r="P6">
-        <v>0.38447589631295526</v>
+        <v>0.81147921936214407</v>
       </c>
       <c r="T6">
         <v>28</v>
       </c>
       <c r="U6">
-        <v>0.67913249851719204</v>
+        <v>0.76977557193192436</v>
       </c>
       <c r="V6">
-        <v>0.32086750148280802</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.23022442806807569</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7">
         <v>29</v>
       </c>
       <c r="B7">
-        <v>0.76168817025837454</v>
+        <v>0.84733845350568238</v>
       </c>
       <c r="C7">
-        <v>0.23831182974162546</v>
+        <v>0.1526615464943176</v>
       </c>
       <c r="H7">
         <v>29</v>
       </c>
       <c r="I7">
-        <v>0.46242077547644395</v>
+        <v>0.38002483683674088</v>
       </c>
       <c r="J7">
-        <v>0.537579224523556</v>
+        <v>0.61997516316325918</v>
       </c>
       <c r="N7">
         <v>29</v>
       </c>
       <c r="O7">
-        <v>0.46242077547644395</v>
+        <v>0.32144763812362981</v>
       </c>
       <c r="P7">
-        <v>0.537579224523556</v>
+        <v>0.67855236187637025</v>
       </c>
       <c r="T7">
         <v>29</v>
       </c>
       <c r="U7">
-        <v>0.71210965519024028</v>
+        <v>0.77698228324638985</v>
       </c>
       <c r="V7">
-        <v>0.28789034480975961</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.22301771675361015</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8">
         <v>30</v>
       </c>
       <c r="B8">
-        <v>0.74474467348577045</v>
+        <v>0.8638401063512634</v>
       </c>
       <c r="C8">
-        <v>0.2552553265142295</v>
+        <v>0.13615989364873654</v>
       </c>
       <c r="H8">
         <v>30</v>
       </c>
       <c r="I8">
-        <v>0.59494311996025107</v>
+        <v>0.40065277807806404</v>
       </c>
       <c r="J8">
-        <v>0.40505688003974899</v>
+        <v>0.5993472219219359</v>
       </c>
       <c r="N8">
         <v>30</v>
       </c>
       <c r="O8">
-        <v>0.59494311996025107</v>
+        <v>0.30478264439729863</v>
       </c>
       <c r="P8">
-        <v>0.40505688003974899</v>
+        <v>0.69521735560270126</v>
       </c>
       <c r="T8">
         <v>30</v>
       </c>
       <c r="U8">
-        <v>0.70595789040125345</v>
+        <v>0.77283425082552049</v>
       </c>
       <c r="V8">
-        <v>0.29404210959874655</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.22716574917447951</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9">
         <v>31</v>
       </c>
       <c r="B9">
-        <v>0.73988418640750053</v>
+        <v>0.85775091610851661</v>
       </c>
       <c r="C9">
-        <v>0.26011581359249941</v>
+        <v>0.14224908389148327</v>
       </c>
       <c r="H9">
         <v>31</v>
       </c>
       <c r="I9">
-        <v>0.48675454875438351</v>
+        <v>0.38053732106263938</v>
       </c>
       <c r="J9">
-        <v>0.51324545124561638</v>
+        <v>0.61946267893736062</v>
       </c>
       <c r="N9">
         <v>31</v>
       </c>
       <c r="O9">
-        <v>0.48675454875438356</v>
+        <v>0.17451785035030165</v>
       </c>
       <c r="P9">
-        <v>0.51324545124561649</v>
+        <v>0.82548214964969835</v>
       </c>
       <c r="T9">
         <v>31</v>
       </c>
       <c r="U9">
-        <v>0.70316043664474148</v>
+        <v>0.78478919227477728</v>
       </c>
       <c r="V9">
-        <v>0.29683956335525852</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.21521080772522272</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10">
         <v>32</v>
       </c>
       <c r="B10">
-        <v>0.78333436569267922</v>
+        <v>0.85664404815889494</v>
       </c>
       <c r="C10">
-        <v>0.2166656343073208</v>
+        <v>0.14335595184110503</v>
       </c>
       <c r="H10">
         <v>32</v>
       </c>
       <c r="I10">
-        <v>0.59118275499921835</v>
+        <v>0.47108405216680532</v>
       </c>
       <c r="J10">
-        <v>0.40881724500078159</v>
+        <v>0.52891594783319462</v>
       </c>
       <c r="N10">
         <v>32</v>
       </c>
       <c r="O10">
-        <v>0.59118275499921835</v>
+        <v>0.22054273529699958</v>
       </c>
       <c r="P10">
-        <v>0.40881724500078159</v>
+        <v>0.77945726470300047</v>
       </c>
       <c r="T10">
         <v>32</v>
       </c>
       <c r="U10">
-        <v>0.70147267221403109</v>
+        <v>0.76208099822598852</v>
       </c>
       <c r="V10">
-        <v>0.29852732778596885</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.23791900177401154</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11">
         <v>33</v>
       </c>
       <c r="B11">
-        <v>0.74017788704825804</v>
+        <v>0.84731293608230529</v>
       </c>
       <c r="C11">
-        <v>0.2598221129517419</v>
+        <v>0.15268706391769471</v>
       </c>
       <c r="H11">
         <v>33</v>
       </c>
       <c r="I11">
-        <v>0.47973761949712485</v>
+        <v>0.35687665535793189</v>
       </c>
       <c r="J11">
-        <v>0.52026238050287521</v>
+        <v>0.64312334464206811</v>
       </c>
       <c r="N11">
         <v>33</v>
       </c>
       <c r="O11">
-        <v>0.47973761949712485</v>
+        <v>0.25181182832838944</v>
       </c>
       <c r="P11">
-        <v>0.52026238050287521</v>
+        <v>0.74818817167161056</v>
       </c>
       <c r="T11">
         <v>33</v>
       </c>
       <c r="U11">
-        <v>0.71873513071592143</v>
+        <v>0.78643712735741933</v>
       </c>
       <c r="V11">
-        <v>0.28126486928407851</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.21356287264258073</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12">
         <v>34</v>
       </c>
       <c r="B12">
-        <v>0.76097913480188328</v>
+        <v>0.85587686536535812</v>
       </c>
       <c r="C12">
-        <v>0.23902086519811669</v>
+        <v>0.1441231346346418</v>
       </c>
       <c r="H12">
         <v>34</v>
       </c>
       <c r="I12">
-        <v>0.57510188540768903</v>
+        <v>0.43778042654786675</v>
       </c>
       <c r="J12">
-        <v>0.42489811459231108</v>
+        <v>0.56221957345213314</v>
       </c>
       <c r="N12">
         <v>34</v>
       </c>
       <c r="O12">
-        <v>0.57510188540768903</v>
+        <v>0.27191637289302445</v>
       </c>
       <c r="P12">
-        <v>0.42489811459231108</v>
+        <v>0.72808362710697561</v>
       </c>
       <c r="T12">
         <v>34</v>
       </c>
       <c r="U12">
-        <v>0.73119262186923828</v>
+        <v>0.79012495440429198</v>
       </c>
       <c r="V12">
-        <v>0.26880737813076178</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.20987504559570802</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13">
         <v>35</v>
       </c>
       <c r="B13">
-        <v>0.76708861112905291</v>
+        <v>0.86535332589934977</v>
       </c>
       <c r="C13">
-        <v>0.23291138887094714</v>
+        <v>0.1346466741006502</v>
       </c>
       <c r="H13">
         <v>35</v>
       </c>
       <c r="I13">
-        <v>0.55679117415248092</v>
+        <v>0.42461608617338231</v>
       </c>
       <c r="J13">
-        <v>0.44320882584751897</v>
+        <v>0.57538391382661769</v>
       </c>
       <c r="N13">
         <v>35</v>
       </c>
       <c r="O13">
-        <v>0.55679117415248103</v>
+        <v>0.34638150836722725</v>
       </c>
       <c r="P13">
-        <v>0.44320882584751903</v>
+        <v>0.65361849163277275</v>
       </c>
       <c r="T13">
         <v>35</v>
       </c>
       <c r="U13">
-        <v>0.73036543370958851</v>
+        <v>0.78170267123913562</v>
       </c>
       <c r="V13">
-        <v>0.26963456629041155</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.21829732876086447</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14">
         <v>36</v>
       </c>
       <c r="B14">
-        <v>0.75894807235844819</v>
+        <v>0.87660198513045695</v>
       </c>
       <c r="C14">
-        <v>0.24105192764155178</v>
+        <v>0.12339801486954309</v>
       </c>
       <c r="H14">
         <v>36</v>
       </c>
       <c r="I14">
-        <v>0.57332584976141976</v>
+        <v>0.43864955384377835</v>
       </c>
       <c r="J14">
-        <v>0.42667415023858019</v>
+        <v>0.56135044615622165</v>
       </c>
       <c r="N14">
         <v>36</v>
       </c>
       <c r="O14">
-        <v>0.57332584976141976</v>
+        <v>0.29035277517603908</v>
       </c>
       <c r="P14">
-        <v>0.42667415023858019</v>
+        <v>0.70964722482396081</v>
       </c>
       <c r="T14">
         <v>36</v>
       </c>
       <c r="U14">
-        <v>0.72464589912272759</v>
+        <v>0.78837615300304353</v>
       </c>
       <c r="V14">
-        <v>0.27535410087727247</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.21162384699695655</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15">
         <v>37</v>
       </c>
       <c r="B15">
-        <v>0.75937115383125464</v>
+        <v>0.87026270089853586</v>
       </c>
       <c r="C15">
-        <v>0.24062884616874528</v>
+        <v>0.12973729910146425</v>
       </c>
       <c r="H15">
         <v>37</v>
       </c>
       <c r="I15">
-        <v>0.57233900699205587</v>
+        <v>0.43879533666671566</v>
       </c>
       <c r="J15">
-        <v>0.42766099300794408</v>
+        <v>0.56120466333328434</v>
       </c>
       <c r="N15">
         <v>37</v>
       </c>
       <c r="O15">
-        <v>0.57233900699205587</v>
+        <v>0.24925048343397257</v>
       </c>
       <c r="P15">
-        <v>0.42766099300794408</v>
+        <v>0.75074951656602751</v>
       </c>
       <c r="T15">
         <v>37</v>
       </c>
       <c r="U15">
-        <v>0.72295680607452562</v>
+        <v>0.7858362350851662</v>
       </c>
       <c r="V15">
-        <v>0.27704319392547438</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.21416376491483391</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16">
         <v>38</v>
       </c>
       <c r="B16">
-        <v>0.76114340050968998</v>
+        <v>0.86479264499437936</v>
       </c>
       <c r="C16">
-        <v>0.23885659949030996</v>
+        <v>0.1352073550056207</v>
       </c>
       <c r="H16">
         <v>38</v>
       </c>
       <c r="I16">
-        <v>0.5360795292675945</v>
+        <v>0.40261529174044819</v>
       </c>
       <c r="J16">
-        <v>0.4639204707324055</v>
+        <v>0.5973847082595517</v>
       </c>
       <c r="N16">
         <v>38</v>
       </c>
       <c r="O16">
-        <v>0.5360795292675945</v>
+        <v>0.30873324667445884</v>
       </c>
       <c r="P16">
-        <v>0.4639204707324055</v>
+        <v>0.69126675332554111</v>
       </c>
       <c r="T16">
         <v>38</v>
       </c>
       <c r="U16">
-        <v>0.729676869163563</v>
+        <v>0.78457226335409846</v>
       </c>
       <c r="V16">
-        <v>0.27032313083643694</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.21542773664590145</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17">
         <v>39</v>
       </c>
       <c r="B17">
-        <v>0.7549011959918267</v>
+        <v>0.8705430367397794</v>
       </c>
       <c r="C17">
-        <v>0.24509880400817333</v>
+        <v>0.12945696326022063</v>
       </c>
       <c r="H17">
         <v>39</v>
       </c>
       <c r="I17">
-        <v>0.53521642171344552</v>
+        <v>0.41260760984041683</v>
       </c>
       <c r="J17">
-        <v>0.46478357828655442</v>
+        <v>0.58739239015958311</v>
       </c>
       <c r="N17">
         <v>39</v>
       </c>
       <c r="O17">
-        <v>0.53521642171344552</v>
+        <v>0.35062943925537354</v>
       </c>
       <c r="P17">
-        <v>0.46478357828655442</v>
+        <v>0.6493705607446264</v>
       </c>
       <c r="T17">
         <v>39</v>
       </c>
       <c r="U17">
-        <v>0.74368583733850613</v>
+        <v>0.79352701221980604</v>
       </c>
       <c r="V17">
-        <v>0.25631416266149398</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.20647298778019391</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18">
         <v>40</v>
       </c>
       <c r="B18">
-        <v>0.7623791730589321</v>
+        <v>0.87439011557987323</v>
       </c>
       <c r="C18">
-        <v>0.2376208269410679</v>
+        <v>0.12560988442012688</v>
       </c>
       <c r="H18">
         <v>40</v>
       </c>
       <c r="I18">
-        <v>0.56106516567052034</v>
+        <v>0.41596195468938324</v>
       </c>
       <c r="J18">
-        <v>0.43893483432947972</v>
+        <v>0.58403804531061687</v>
       </c>
       <c r="N18">
         <v>40</v>
       </c>
       <c r="O18">
-        <v>0.56106516567052034</v>
+        <v>0.29617332634299259</v>
       </c>
       <c r="P18">
-        <v>0.43893483432947972</v>
+        <v>0.70382667365700735</v>
       </c>
       <c r="T18">
         <v>40</v>
       </c>
       <c r="U18">
-        <v>0.76152603972266619</v>
+        <v>0.82303248300873932</v>
       </c>
       <c r="V18">
-        <v>0.23847396027733381</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.17696751699126068</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19">
         <v>41</v>
       </c>
       <c r="B19">
-        <v>0.76096252025082556</v>
+        <v>0.86043290398143446</v>
       </c>
       <c r="C19">
-        <v>0.23903747974917441</v>
+        <v>0.13956709601856554</v>
       </c>
       <c r="H19">
         <v>41</v>
       </c>
       <c r="I19">
-        <v>0.56057375392423059</v>
+        <v>0.42277551630385524</v>
       </c>
       <c r="J19">
-        <v>0.43942624607576947</v>
+        <v>0.57722448369614476</v>
       </c>
       <c r="N19">
         <v>41</v>
       </c>
       <c r="O19">
-        <v>0.56057375392423059</v>
+        <v>0.23986285454067924</v>
       </c>
       <c r="P19">
-        <v>0.43942624607576947</v>
+        <v>0.76013714545932087</v>
       </c>
       <c r="T19">
         <v>41</v>
       </c>
       <c r="U19">
-        <v>0.76465597039242861</v>
+        <v>0.82435037676105294</v>
       </c>
       <c r="V19">
-        <v>0.23534402960757136</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.17564962323894703</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20">
         <v>42</v>
       </c>
       <c r="B20">
-        <v>0.7552696792781346</v>
+        <v>0.84948991742747637</v>
       </c>
       <c r="C20">
-        <v>0.24473032072186537</v>
+        <v>0.15051008257252368</v>
       </c>
       <c r="H20">
         <v>42</v>
       </c>
       <c r="I20">
-        <v>0.50700638836685508</v>
+        <v>0.38776856331023657</v>
       </c>
       <c r="J20">
-        <v>0.49299361163314498</v>
+        <v>0.61223143668976343</v>
       </c>
       <c r="N20">
         <v>42</v>
       </c>
       <c r="O20">
-        <v>0.50700638836685508</v>
+        <v>0.31229632190970419</v>
       </c>
       <c r="P20">
-        <v>0.49299361163314498</v>
+        <v>0.68770367809029576</v>
       </c>
       <c r="T20">
         <v>42</v>
       </c>
       <c r="U20">
-        <v>0.75740380000703966</v>
+        <v>0.80670108638972349</v>
       </c>
       <c r="V20">
-        <v>0.24259619999296034</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.19329891361027654</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21">
         <v>43</v>
       </c>
       <c r="B21">
-        <v>0.74126324314143988</v>
+        <v>0.84706799450425552</v>
       </c>
       <c r="C21">
-        <v>0.25873675685856018</v>
+        <v>0.15293200549574451</v>
       </c>
       <c r="H21">
         <v>43</v>
       </c>
       <c r="I21">
-        <v>0.49197758438986039</v>
+        <v>0.36850038246576622</v>
       </c>
       <c r="J21">
-        <v>0.50802241561013961</v>
+        <v>0.63149961753423367</v>
       </c>
       <c r="N21">
         <v>43</v>
       </c>
       <c r="O21">
-        <v>0.49197758438986039</v>
+        <v>0.23884701823088497</v>
       </c>
       <c r="P21">
-        <v>0.50802241561013961</v>
+        <v>0.76115298176911506</v>
       </c>
       <c r="T21">
         <v>43</v>
       </c>
       <c r="U21">
-        <v>0.75814041422089662</v>
+        <v>0.81564232740318277</v>
       </c>
       <c r="V21">
-        <v>0.24185958577910333</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.18435767259681726</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22">
         <v>44</v>
       </c>
       <c r="B22">
-        <v>0.71828399776448004</v>
+        <v>0.83593024208217692</v>
       </c>
       <c r="C22">
-        <v>0.28171600223551996</v>
+        <v>0.16406975791782313</v>
       </c>
       <c r="H22">
         <v>44</v>
       </c>
       <c r="I22">
-        <v>0.57929919906664995</v>
+        <v>0.4155020554318184</v>
       </c>
       <c r="J22">
-        <v>0.42070080093335005</v>
+        <v>0.58449794456818172</v>
       </c>
       <c r="N22">
         <v>44</v>
       </c>
       <c r="O22">
-        <v>0.57929919906664995</v>
+        <v>0.3350503611712109</v>
       </c>
       <c r="P22">
-        <v>0.42070080093335005</v>
+        <v>0.6649496388287891</v>
       </c>
       <c r="T22">
         <v>44</v>
       </c>
       <c r="U22">
-        <v>0.76720334579753269</v>
+        <v>0.81416166714340543</v>
       </c>
       <c r="V22">
-        <v>0.23279665420246734</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.18583833285659465</v>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23">
         <v>45</v>
       </c>
       <c r="B23">
-        <v>0.74275328287954512</v>
+        <v>0.85070866375718712</v>
       </c>
       <c r="C23">
-        <v>0.25724671712045483</v>
+        <v>0.14929133624281288</v>
       </c>
       <c r="H23">
         <v>45</v>
       </c>
       <c r="I23">
-        <v>0.54589053097319473</v>
+        <v>0.44412031079816711</v>
       </c>
       <c r="J23">
-        <v>0.45410946902680521</v>
+        <v>0.55587968920183284</v>
       </c>
       <c r="N23">
         <v>45</v>
       </c>
       <c r="O23">
-        <v>0.54589053097319473</v>
+        <v>0.26099126309845583</v>
       </c>
       <c r="P23">
-        <v>0.45410946902680521</v>
+        <v>0.73900873690154412</v>
       </c>
       <c r="T23">
         <v>45</v>
       </c>
       <c r="U23">
-        <v>0.75457119423721108</v>
+        <v>0.81100361344969729</v>
       </c>
       <c r="V23">
-        <v>0.24542880576278889</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.18899638655030271</v>
+      </c>
+    </row>
+    <row r="24">
       <c r="A24">
         <v>46</v>
       </c>
       <c r="B24">
-        <v>0.74511012100584206</v>
+        <v>0.84886742994928488</v>
       </c>
       <c r="C24">
-        <v>0.25488987899415799</v>
+        <v>0.15113257005071518</v>
       </c>
       <c r="H24">
         <v>46</v>
       </c>
       <c r="I24">
-        <v>0.55360777004113104</v>
+        <v>0.45754754486056914</v>
       </c>
       <c r="J24">
-        <v>0.44639222995886901</v>
+        <v>0.54245245513943074</v>
       </c>
       <c r="N24">
         <v>46</v>
       </c>
       <c r="O24">
-        <v>0.55360777004113104</v>
+        <v>0.31971630050134636</v>
       </c>
       <c r="P24">
-        <v>0.44639222995886901</v>
+        <v>0.68028369949865375</v>
       </c>
       <c r="T24">
         <v>46</v>
       </c>
       <c r="U24">
-        <v>0.75646302811820254</v>
+        <v>0.80640921221095985</v>
       </c>
       <c r="V24">
-        <v>0.24353697188179749</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.19359078778904007</v>
+      </c>
+    </row>
+    <row r="25">
       <c r="A25">
         <v>47</v>
       </c>
       <c r="B25">
-        <v>0.70642752273856724</v>
+        <v>0.83944495126579977</v>
       </c>
       <c r="C25">
-        <v>0.29357247726143271</v>
+        <v>0.16055504873420021</v>
       </c>
       <c r="H25">
         <v>47</v>
       </c>
       <c r="I25">
-        <v>0.45581192339807941</v>
+        <v>0.33280742113103734</v>
       </c>
       <c r="J25">
-        <v>0.54418807660192059</v>
+        <v>0.66719257886896277</v>
       </c>
       <c r="N25">
         <v>47</v>
       </c>
       <c r="O25">
-        <v>0.45581192339807941</v>
+        <v>0.29173869110825401</v>
       </c>
       <c r="P25">
-        <v>0.54418807660192059</v>
+        <v>0.70826130889174599</v>
       </c>
       <c r="T25">
         <v>47</v>
       </c>
       <c r="U25">
-        <v>0.76145539111185878</v>
+        <v>0.8145122132383531</v>
       </c>
       <c r="V25">
-        <v>0.23854460888814125</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.18548778676164684</v>
+      </c>
+    </row>
+    <row r="26">
       <c r="A26">
         <v>48</v>
       </c>
       <c r="B26">
-        <v>0.73146981340373474</v>
+        <v>0.85297101004791309</v>
       </c>
       <c r="C26">
-        <v>0.26853018659626537</v>
+        <v>0.14702898995208688</v>
       </c>
       <c r="H26">
         <v>48</v>
       </c>
       <c r="I26">
-        <v>0.48016486603653308</v>
+        <v>0.37773759933749596</v>
       </c>
       <c r="J26">
-        <v>0.51983513396346692</v>
+        <v>0.62226240066250393</v>
       </c>
       <c r="N26">
         <v>48</v>
       </c>
       <c r="O26">
-        <v>0.48016486603653308</v>
+        <v>0.2378981645048952</v>
       </c>
       <c r="P26">
-        <v>0.51983513396346692</v>
+        <v>0.7621018354951048</v>
       </c>
       <c r="T26">
         <v>48</v>
       </c>
       <c r="U26">
-        <v>0.75961519453111093</v>
+        <v>0.81169744672528032</v>
       </c>
       <c r="V26">
-        <v>0.24038480546888905</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.18830255327471965</v>
+      </c>
+    </row>
+    <row r="27">
       <c r="A27">
         <v>49</v>
       </c>
       <c r="B27">
-        <v>0.71702088732630387</v>
+        <v>0.85523735284625169</v>
       </c>
       <c r="C27">
-        <v>0.28297911267369608</v>
+        <v>0.14476264715374831</v>
       </c>
       <c r="H27">
         <v>49</v>
       </c>
       <c r="I27">
-        <v>0.49201430600068258</v>
+        <v>0.35435746259444695</v>
       </c>
       <c r="J27">
-        <v>0.50798569399931737</v>
+        <v>0.645642537405553</v>
       </c>
       <c r="N27">
         <v>49</v>
       </c>
       <c r="O27">
-        <v>0.49201430600068258</v>
+        <v>0.32149898989496783</v>
       </c>
       <c r="P27">
-        <v>0.50798569399931737</v>
+        <v>0.67850101010503205</v>
       </c>
       <c r="T27">
         <v>49</v>
       </c>
       <c r="U27">
-        <v>0.77569600811034489</v>
+        <v>0.81742900099179538</v>
       </c>
       <c r="V27">
-        <v>0.22430399188965511</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.18257099900820464</v>
+      </c>
+    </row>
+    <row r="28">
       <c r="A28">
         <v>50</v>
       </c>
       <c r="B28">
-        <v>0.74102266640002956</v>
+        <v>0.85166773682366104</v>
       </c>
       <c r="C28">
-        <v>0.25897733359997044</v>
+        <v>0.14833226317633888</v>
       </c>
       <c r="H28">
         <v>50</v>
       </c>
       <c r="I28">
-        <v>0.51251890921860543</v>
+        <v>0.41359984262553884</v>
       </c>
       <c r="J28">
-        <v>0.48748109078139457</v>
+        <v>0.58640015737446127</v>
       </c>
       <c r="N28">
         <v>50</v>
       </c>
       <c r="O28">
-        <v>0.51251890921860543</v>
+        <v>0.22249908709768457</v>
       </c>
       <c r="P28">
-        <v>0.48748109078139457</v>
+        <v>0.77750091290231549</v>
       </c>
       <c r="T28">
         <v>50</v>
       </c>
       <c r="U28">
-        <v>0.75784346563266813</v>
+        <v>0.81566785046289181</v>
       </c>
       <c r="V28">
-        <v>0.24215653436733184</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.18433214953710816</v>
+      </c>
+    </row>
+    <row r="29">
       <c r="A29">
         <v>51</v>
       </c>
       <c r="B29">
-        <v>0.74451604236558766</v>
+        <v>0.88024643766294264</v>
       </c>
       <c r="C29">
-        <v>0.25548395763441234</v>
+        <v>0.11975356233705745</v>
       </c>
       <c r="H29">
         <v>51</v>
       </c>
       <c r="I29">
-        <v>0.5291852010636986</v>
+        <v>0.39914091855054801</v>
       </c>
       <c r="J29">
-        <v>0.47081479893630129</v>
+        <v>0.60085908144945199</v>
       </c>
       <c r="N29">
         <v>51</v>
       </c>
       <c r="O29">
-        <v>0.52918520106369871</v>
+        <v>0.31196176980399332</v>
       </c>
       <c r="P29">
-        <v>0.47081479893630135</v>
+        <v>0.68803823019600674</v>
       </c>
       <c r="T29">
         <v>51</v>
       </c>
       <c r="U29">
-        <v>0.78754095967555748</v>
+        <v>0.83373935100438223</v>
       </c>
       <c r="V29">
-        <v>0.21245904032444246</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.16626064899561771</v>
+      </c>
+    </row>
+    <row r="30">
       <c r="A30">
         <v>52</v>
       </c>
       <c r="B30">
-        <v>0.72677974591597971</v>
+        <v>0.83472390137699326</v>
       </c>
       <c r="C30">
-        <v>0.27322025408402029</v>
+        <v>0.16527609862300671</v>
       </c>
       <c r="H30">
         <v>52</v>
       </c>
       <c r="I30">
-        <v>0.47682374050499027</v>
+        <v>0.3915677642124219</v>
       </c>
       <c r="J30">
-        <v>0.52317625949500979</v>
+        <v>0.6084322357875781</v>
       </c>
       <c r="N30">
         <v>52</v>
       </c>
       <c r="O30">
-        <v>0.47682374050499027</v>
+        <v>0.27061031771008104</v>
       </c>
       <c r="P30">
-        <v>0.52317625949500979</v>
+        <v>0.72938968228991896</v>
       </c>
       <c r="T30">
         <v>52</v>
       </c>
       <c r="U30">
-        <v>0.77632975413339367</v>
+        <v>0.8233256449376718</v>
       </c>
       <c r="V30">
-        <v>0.22367024586660633</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.17667435506232815</v>
+      </c>
+    </row>
+    <row r="31">
       <c r="A31">
         <v>53</v>
       </c>
       <c r="B31">
-        <v>0.7486146737200674</v>
+        <v>0.87839797478307635</v>
       </c>
       <c r="C31">
-        <v>0.2513853262799326</v>
+        <v>0.12160202521692363</v>
       </c>
       <c r="H31">
         <v>53</v>
       </c>
       <c r="I31">
-        <v>0.52964856436182484</v>
+        <v>0.40362625438213789</v>
       </c>
       <c r="J31">
-        <v>0.47035143563817522</v>
+        <v>0.59637374561786216</v>
       </c>
       <c r="N31">
         <v>53</v>
       </c>
       <c r="O31">
-        <v>0.52964856436182484</v>
+        <v>0.27215100171922241</v>
       </c>
       <c r="P31">
-        <v>0.47035143563817522</v>
+        <v>0.72784899828077765</v>
       </c>
       <c r="T31">
         <v>53</v>
       </c>
       <c r="U31">
-        <v>0.78892191654158905</v>
+        <v>0.84659782549519835</v>
       </c>
       <c r="V31">
-        <v>0.21107808345841092</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.15340217450480167</v>
+      </c>
+    </row>
+    <row r="32">
       <c r="A32">
         <v>54</v>
       </c>
       <c r="B32">
-        <v>0.77808932660710173</v>
+        <v>0.87950821855950212</v>
       </c>
       <c r="C32">
-        <v>0.22191067339289838</v>
+        <v>0.12049178144049791</v>
       </c>
       <c r="H32">
         <v>54</v>
       </c>
       <c r="I32">
-        <v>0.50479919842736409</v>
+        <v>0.40670359745864654</v>
       </c>
       <c r="J32">
-        <v>0.49520080157263591</v>
+        <v>0.59329640254135352</v>
       </c>
       <c r="N32">
         <v>54</v>
       </c>
       <c r="O32">
-        <v>0.50479919842736409</v>
+        <v>0.2848790572551439</v>
       </c>
       <c r="P32">
-        <v>0.49520080157263591</v>
+        <v>0.71512094274485616</v>
       </c>
       <c r="T32">
         <v>54</v>
       </c>
       <c r="U32">
-        <v>0.77911911326124006</v>
+        <v>0.82439613788670441</v>
       </c>
       <c r="V32">
-        <v>0.22088088673875997</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.17560386211329562</v>
+      </c>
+    </row>
+    <row r="33">
       <c r="A33">
         <v>55</v>
       </c>
       <c r="B33">
-        <v>0.75286315756453714</v>
+        <v>0.85739533018574088</v>
       </c>
       <c r="C33">
-        <v>0.2471368424354628</v>
+        <v>0.14260466981425901</v>
       </c>
       <c r="H33">
         <v>55</v>
       </c>
       <c r="I33">
-        <v>0.47859288463042404</v>
+        <v>0.39169695956001266</v>
       </c>
       <c r="J33">
-        <v>0.52140711536957596</v>
+        <v>0.60830304043998729</v>
       </c>
       <c r="N33">
         <v>55</v>
       </c>
       <c r="O33">
-        <v>0.47859288463042404</v>
+        <v>0.32422422722840444</v>
       </c>
       <c r="P33">
-        <v>0.52140711536957596</v>
+        <v>0.67577577277159562</v>
       </c>
       <c r="T33">
         <v>55</v>
       </c>
       <c r="U33">
-        <v>0.79101345554349445</v>
+        <v>0.83104558981707211</v>
       </c>
       <c r="V33">
-        <v>0.20898654445650555</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.16895441018292792</v>
+      </c>
+    </row>
+    <row r="34">
       <c r="A34">
         <v>56</v>
       </c>
       <c r="B34">
-        <v>0.73622499576984068</v>
+        <v>0.87228754292915844</v>
       </c>
       <c r="C34">
-        <v>0.26377500423015932</v>
+        <v>0.12771245707084158</v>
       </c>
       <c r="H34">
         <v>56</v>
       </c>
       <c r="I34">
-        <v>0.53543442601005076</v>
+        <v>0.36601610997605316</v>
       </c>
       <c r="J34">
-        <v>0.46456557398994924</v>
+        <v>0.63398389002394673</v>
       </c>
       <c r="N34">
         <v>56</v>
       </c>
       <c r="O34">
-        <v>0.53543442601005076</v>
+        <v>0.32263686244651468</v>
       </c>
       <c r="P34">
-        <v>0.46456557398994924</v>
+        <v>0.67736313755348532</v>
       </c>
       <c r="T34">
         <v>56</v>
       </c>
       <c r="U34">
-        <v>0.79222996238492782</v>
+        <v>0.83641938750793388</v>
       </c>
       <c r="V34">
-        <v>0.20777003761507218</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.1635806124920661</v>
+      </c>
+    </row>
+    <row r="35">
       <c r="A35">
         <v>57</v>
       </c>
       <c r="B35">
-        <v>0.74682203395280655</v>
+        <v>0.86106173457017532</v>
       </c>
       <c r="C35">
-        <v>0.25317796604719339</v>
+        <v>0.13893826542982471</v>
       </c>
       <c r="H35">
         <v>57</v>
       </c>
       <c r="I35">
-        <v>0.50360997875985913</v>
+        <v>0.40828431423230471</v>
       </c>
       <c r="J35">
-        <v>0.49639002124014087</v>
+        <v>0.59171568576769529</v>
       </c>
       <c r="N35">
         <v>57</v>
       </c>
       <c r="O35">
-        <v>0.50360997875985913</v>
+        <v>0.2505818437207758</v>
       </c>
       <c r="P35">
-        <v>0.49639002124014087</v>
+        <v>0.74941815627922415</v>
       </c>
       <c r="T35">
         <v>57</v>
       </c>
       <c r="U35">
-        <v>0.81160900822571558</v>
+        <v>0.86042422340538949</v>
       </c>
       <c r="V35">
-        <v>0.18839099177428437</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.13957577659461054</v>
+      </c>
+    </row>
+    <row r="36">
       <c r="A36">
         <v>58</v>
       </c>
       <c r="B36">
-        <v>0.72641128619910555</v>
+        <v>0.86212724333460455</v>
       </c>
       <c r="C36">
-        <v>0.2735887138008945</v>
+        <v>0.13787275666539547</v>
       </c>
       <c r="H36">
         <v>58</v>
       </c>
       <c r="I36">
-        <v>0.47236548058496325</v>
+        <v>0.37093786181075</v>
       </c>
       <c r="J36">
-        <v>0.5276345194150367</v>
+        <v>0.62906213818924994</v>
       </c>
       <c r="N36">
         <v>58</v>
       </c>
       <c r="O36">
-        <v>0.47236548058496325</v>
+        <v>0.26729505686754013</v>
       </c>
       <c r="P36">
-        <v>0.5276345194150367</v>
+        <v>0.73270494313245993</v>
       </c>
       <c r="T36">
         <v>58</v>
       </c>
       <c r="U36">
-        <v>0.80594812819079509</v>
+        <v>0.84602591911032954</v>
       </c>
       <c r="V36">
-        <v>0.19405187180920494</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.15397408088967052</v>
+      </c>
+    </row>
+    <row r="37">
       <c r="A37">
         <v>59</v>
       </c>
       <c r="B37">
-        <v>0.73701090442855799</v>
+        <v>0.86003785623028572</v>
       </c>
       <c r="C37">
-        <v>0.26298909557144196</v>
+        <v>0.13996214376971425</v>
       </c>
       <c r="H37">
         <v>59</v>
       </c>
       <c r="I37">
-        <v>0.49430905752864696</v>
+        <v>0.4037748331612025</v>
       </c>
       <c r="J37">
-        <v>0.50569094247135304</v>
+        <v>0.59622516683879756</v>
       </c>
       <c r="N37">
         <v>59</v>
       </c>
       <c r="O37">
-        <v>0.49430905752864696</v>
+        <v>0.28954711466858724</v>
       </c>
       <c r="P37">
-        <v>0.50569094247135304</v>
+        <v>0.71045288533141282</v>
       </c>
       <c r="T37">
         <v>59</v>
       </c>
       <c r="U37">
-        <v>0.7995677107554221</v>
+        <v>0.83322713978533003</v>
       </c>
       <c r="V37">
-        <v>0.20043228924457795</v>
-      </c>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.16677286021467005</v>
+      </c>
+    </row>
+    <row r="38">
       <c r="A38">
         <v>60</v>
       </c>
       <c r="B38">
-        <v>0.73878548275216949</v>
+        <v>0.85322248454475302</v>
       </c>
       <c r="C38">
-        <v>0.26121451724783051</v>
+        <v>0.14677751545524703</v>
       </c>
       <c r="H38">
         <v>60</v>
       </c>
       <c r="I38">
-        <v>0.44847130372704047</v>
+        <v>0.40949481249937136</v>
       </c>
       <c r="J38">
-        <v>0.55152869627295964</v>
+        <v>0.59050518750062864</v>
       </c>
       <c r="N38">
         <v>60</v>
       </c>
       <c r="O38">
-        <v>0.44847130372704047</v>
+        <v>0.3062447429428139</v>
       </c>
       <c r="P38">
-        <v>0.55152869627295964</v>
+        <v>0.69375525705718621</v>
       </c>
       <c r="T38">
         <v>60</v>
       </c>
       <c r="U38">
-        <v>0.82253090780869142</v>
+        <v>0.85583183635213922</v>
       </c>
       <c r="V38">
-        <v>0.17746909219130866</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.14416816364786075</v>
+      </c>
+    </row>
+    <row r="39">
       <c r="A39">
         <v>61</v>
       </c>
       <c r="B39">
-        <v>0.71573915284245604</v>
+        <v>0.84998765135052923</v>
       </c>
       <c r="C39">
-        <v>0.28426084715754391</v>
+        <v>0.1500123486494708</v>
       </c>
       <c r="H39">
         <v>61</v>
       </c>
       <c r="I39">
-        <v>0.49289506085966928</v>
+        <v>0.38896417708499653</v>
       </c>
       <c r="J39">
-        <v>0.50710493914033072</v>
+        <v>0.61103582291500336</v>
       </c>
       <c r="N39">
         <v>61</v>
       </c>
       <c r="O39">
-        <v>0.49289506085966928</v>
+        <v>0.30332949025461164</v>
       </c>
       <c r="P39">
-        <v>0.50710493914033072</v>
+        <v>0.69667050974538836</v>
       </c>
       <c r="T39">
         <v>61</v>
       </c>
       <c r="U39">
-        <v>0.82122768570668903</v>
+        <v>0.85467298573152961</v>
       </c>
       <c r="V39">
-        <v>0.17877231429331089</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.14532701426847039</v>
+      </c>
+    </row>
+    <row r="40">
       <c r="A40">
         <v>62</v>
       </c>
       <c r="B40">
-        <v>0.71487316607736129</v>
+        <v>0.87181059798245863</v>
       </c>
       <c r="C40">
-        <v>0.28512683392263871</v>
+        <v>0.12818940201754137</v>
       </c>
       <c r="H40">
         <v>62</v>
       </c>
       <c r="I40">
-        <v>0.49507505106906829</v>
+        <v>0.38308859914801358</v>
       </c>
       <c r="J40">
-        <v>0.50492494893093176</v>
+        <v>0.61691140085198648</v>
       </c>
       <c r="N40">
         <v>62</v>
       </c>
       <c r="O40">
-        <v>0.49507505106906829</v>
+        <v>0.29719406615830629</v>
       </c>
       <c r="P40">
-        <v>0.50492494893093176</v>
+        <v>0.70280593384169376</v>
       </c>
       <c r="T40">
         <v>62</v>
       </c>
       <c r="U40">
-        <v>0.83334629648895653</v>
+        <v>0.86691667206327561</v>
       </c>
       <c r="V40">
-        <v>0.16665370351104353</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.13308332793672428</v>
+      </c>
+    </row>
+    <row r="41">
       <c r="A41">
         <v>63</v>
       </c>
       <c r="B41">
-        <v>0.73286088928694082</v>
+        <v>0.88656404554817192</v>
       </c>
       <c r="C41">
-        <v>0.26713911071305912</v>
+        <v>0.11343595445182811</v>
       </c>
       <c r="H41">
         <v>63</v>
       </c>
       <c r="I41">
-        <v>0.47172276971757177</v>
+        <v>0.36656705881430607</v>
       </c>
       <c r="J41">
-        <v>0.52827723028242823</v>
+        <v>0.63343294118569393</v>
       </c>
       <c r="N41">
         <v>63</v>
       </c>
       <c r="O41">
-        <v>0.47172276971757177</v>
+        <v>0.19932539841315877</v>
       </c>
       <c r="P41">
-        <v>0.52827723028242823</v>
+        <v>0.80067460158684112</v>
       </c>
       <c r="T41">
         <v>63</v>
       </c>
       <c r="U41">
-        <v>0.83424409916613118</v>
+        <v>0.86706949290065805</v>
       </c>
       <c r="V41">
-        <v>0.16575590083386879</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.13293050709934195</v>
+      </c>
+    </row>
+    <row r="42">
       <c r="A42">
         <v>64</v>
       </c>
       <c r="B42">
-        <v>0.66540532516906126</v>
+        <v>0.81927843129139422</v>
       </c>
       <c r="C42">
-        <v>0.3345946748309388</v>
+        <v>0.18072156870860587</v>
       </c>
       <c r="H42">
         <v>64</v>
       </c>
       <c r="I42">
-        <v>0.49220495623278937</v>
+        <v>0.35214059788009816</v>
       </c>
       <c r="J42">
-        <v>0.50779504376721063</v>
+        <v>0.64785940211990189</v>
       </c>
       <c r="N42">
         <v>64</v>
       </c>
       <c r="O42">
-        <v>0.49220495623278937</v>
+        <v>0.35849468263281997</v>
       </c>
       <c r="P42">
-        <v>0.50779504376721063</v>
+        <v>0.64150531736717997</v>
       </c>
       <c r="T42">
         <v>64</v>
       </c>
       <c r="U42">
-        <v>0.85377493292194806</v>
+        <v>0.87387547208295002</v>
       </c>
       <c r="V42">
-        <v>0.14622506707805197</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.12612452791704998</v>
+      </c>
+    </row>
+    <row r="43">
       <c r="A43">
         <v>65</v>
       </c>
       <c r="B43">
-        <v>0.67097759044068983</v>
+        <v>0.86843454229518435</v>
       </c>
       <c r="C43">
-        <v>0.32902240955931028</v>
+        <v>0.13156545770481567</v>
       </c>
       <c r="H43">
         <v>65</v>
       </c>
       <c r="I43">
-        <v>0.42801308174386121</v>
+        <v>0.29884290842599182</v>
       </c>
       <c r="J43">
-        <v>0.57198691825613879</v>
+        <v>0.70115709157400807</v>
       </c>
       <c r="N43">
         <v>65</v>
       </c>
       <c r="O43">
-        <v>0.42801308174386121</v>
+        <v>0.30739433126140997</v>
       </c>
       <c r="P43">
-        <v>0.57198691825613879</v>
+        <v>0.69260566873858997</v>
       </c>
       <c r="T43">
         <v>65</v>
       </c>
       <c r="U43">
-        <v>0.84497785464963138</v>
+        <v>0.875890643360143</v>
       </c>
       <c r="V43">
-        <v>0.15502214535036865</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.12410935663985706</v>
+      </c>
+    </row>
+    <row r="44">
       <c r="A44">
         <v>66</v>
       </c>
       <c r="B44">
-        <v>0.69919558725444408</v>
+        <v>0.86583262153772211</v>
       </c>
       <c r="C44">
-        <v>0.30080441274555597</v>
+        <v>0.13416737846227789</v>
       </c>
       <c r="H44">
         <v>66</v>
       </c>
       <c r="I44">
-        <v>0.5037243273435914</v>
+        <v>0.3778557119593528</v>
       </c>
       <c r="J44">
-        <v>0.4962756726564086</v>
+        <v>0.62214428804064714</v>
       </c>
       <c r="N44">
         <v>66</v>
       </c>
       <c r="O44">
-        <v>0.5037243273435914</v>
+        <v>0.25119319271276486</v>
       </c>
       <c r="P44">
-        <v>0.4962756726564086</v>
+        <v>0.74880680728723503</v>
       </c>
       <c r="T44">
         <v>66</v>
       </c>
       <c r="U44">
-        <v>0.853830685170899</v>
+        <v>0.88049362070908777</v>
       </c>
       <c r="V44">
-        <v>0.14616931482910103</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.11950637929091235</v>
+      </c>
+    </row>
+    <row r="45">
       <c r="A45">
         <v>67</v>
       </c>
       <c r="B45">
-        <v>0.66715437945576384</v>
+        <v>0.86237824493402793</v>
       </c>
       <c r="C45">
-        <v>0.33284562054423616</v>
+        <v>0.13762175506597221</v>
       </c>
       <c r="H45">
         <v>67</v>
       </c>
       <c r="I45">
-        <v>0.4734869177914417</v>
+        <v>0.34590733315213584</v>
       </c>
       <c r="J45">
-        <v>0.52651308220855841</v>
+        <v>0.65409266684786416</v>
       </c>
       <c r="N45">
         <v>67</v>
       </c>
       <c r="O45">
-        <v>0.4734869177914417</v>
+        <v>0.31728046678266197</v>
       </c>
       <c r="P45">
-        <v>0.52651308220855841</v>
+        <v>0.68271953321733814</v>
       </c>
       <c r="T45">
         <v>67</v>
       </c>
       <c r="U45">
-        <v>0.85534161934719688</v>
+        <v>0.87497567331765969</v>
       </c>
       <c r="V45">
-        <v>0.14465838065280312</v>
-      </c>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.12502432668234031</v>
+      </c>
+    </row>
+    <row r="46">
       <c r="A46">
         <v>68</v>
       </c>
       <c r="B46">
-        <v>0.64070835529748782</v>
+        <v>0.85019651152380527</v>
       </c>
       <c r="C46">
-        <v>0.35929164470251213</v>
+        <v>0.14980348847619479</v>
       </c>
       <c r="H46">
         <v>68</v>
       </c>
       <c r="I46">
-        <v>0.4106496135338662</v>
+        <v>0.30808878518837662</v>
       </c>
       <c r="J46">
-        <v>0.58935038646613391</v>
+        <v>0.69191121481162332</v>
       </c>
       <c r="N46">
         <v>68</v>
       </c>
       <c r="O46">
-        <v>0.4106496135338662</v>
+        <v>0.24258895450369605</v>
       </c>
       <c r="P46">
-        <v>0.58935038646613391</v>
+        <v>0.757411045496304</v>
       </c>
       <c r="T46">
         <v>68</v>
       </c>
       <c r="U46">
-        <v>0.85134457802298646</v>
+        <v>0.87532230895221985</v>
       </c>
       <c r="V46">
-        <v>0.14865542197701345</v>
-      </c>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.12467769104778005</v>
+      </c>
+    </row>
+    <row r="47">
       <c r="A47">
         <v>69</v>
       </c>
       <c r="B47">
-        <v>0.69951395016792917</v>
+        <v>0.87277653684604195</v>
       </c>
       <c r="C47">
-        <v>0.30048604983207089</v>
+        <v>0.12722346315395808</v>
       </c>
       <c r="H47">
         <v>69</v>
       </c>
       <c r="I47">
-        <v>0.42310857945425323</v>
+        <v>0.3609802330353315</v>
       </c>
       <c r="J47">
-        <v>0.57689142054574682</v>
+        <v>0.63901976696466845</v>
       </c>
       <c r="N47">
         <v>69</v>
       </c>
       <c r="O47">
-        <v>0.42310857945425323</v>
+        <v>0.26318745950578426</v>
       </c>
       <c r="P47">
-        <v>0.57689142054574682</v>
+        <v>0.73681254049421585</v>
       </c>
       <c r="T47">
         <v>69</v>
       </c>
       <c r="U47">
-        <v>0.82720327889494305</v>
+        <v>0.85116386815479717</v>
       </c>
       <c r="V47">
-        <v>0.17279672110505701</v>
-      </c>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.14883613184520289</v>
+      </c>
+    </row>
+    <row r="48">
       <c r="A48">
         <v>70</v>
       </c>
       <c r="B48">
-        <v>0.64062932697017805</v>
+        <v>0.85142688240008457</v>
       </c>
       <c r="C48">
-        <v>0.35937067302982195</v>
+        <v>0.14857311759991537</v>
       </c>
       <c r="H48">
         <v>70</v>
       </c>
       <c r="I48">
-        <v>0.41961482145517659</v>
+        <v>0.33288221829899672</v>
       </c>
       <c r="J48">
-        <v>0.58038517854482341</v>
+        <v>0.66711778170100322</v>
       </c>
       <c r="N48">
         <v>70</v>
       </c>
       <c r="O48">
-        <v>0.41961482145517659</v>
+        <v>0.18658803494375623</v>
       </c>
       <c r="P48">
-        <v>0.58038517854482341</v>
+        <v>0.81341196505624369</v>
       </c>
       <c r="T48">
         <v>70</v>
       </c>
       <c r="U48">
-        <v>0.84245069185237986</v>
+        <v>0.86657568385077932</v>
       </c>
       <c r="V48">
-        <v>0.15754930814762017</v>
-      </c>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.13342431614922062</v>
+      </c>
+    </row>
+    <row r="49">
       <c r="A49">
         <v>71</v>
       </c>
       <c r="B49">
-        <v>0.66613805025826833</v>
+        <v>0.84909152218767625</v>
       </c>
       <c r="C49">
-        <v>0.33386194974173161</v>
+        <v>0.15090847781232375</v>
       </c>
       <c r="H49">
         <v>71</v>
       </c>
       <c r="I49">
-        <v>0.42224002020019347</v>
+        <v>0.37066614956492144</v>
       </c>
       <c r="J49">
-        <v>0.57775997979980664</v>
+        <v>0.62933385043507861</v>
       </c>
       <c r="N49">
         <v>71</v>
       </c>
       <c r="O49">
-        <v>0.42224002020019347</v>
+        <v>0.32462452159561617</v>
       </c>
       <c r="P49">
-        <v>0.57775997979980664</v>
+        <v>0.67537547840438394</v>
       </c>
       <c r="T49">
         <v>71</v>
       </c>
       <c r="U49">
-        <v>0.83987874583767264</v>
+        <v>0.85819412173868292</v>
       </c>
       <c r="V49">
-        <v>0.16012125416232731</v>
-      </c>
-    </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.14180587826131705</v>
+      </c>
+    </row>
+    <row r="50">
       <c r="A50">
         <v>72</v>
       </c>
       <c r="B50">
-        <v>0.58947887348878114</v>
+        <v>0.82202584326514605</v>
       </c>
       <c r="C50">
-        <v>0.41052112651121875</v>
+        <v>0.17797415673485401</v>
       </c>
       <c r="H50">
         <v>72</v>
       </c>
       <c r="I50">
-        <v>0.48317745028435216</v>
+        <v>0.35371390762291449</v>
       </c>
       <c r="J50">
-        <v>0.51682254971564778</v>
+        <v>0.64628609237708545</v>
       </c>
       <c r="N50">
         <v>72</v>
       </c>
       <c r="O50">
-        <v>0.48317745028435216</v>
+        <v>0.2240481153856474</v>
       </c>
       <c r="P50">
-        <v>0.51682254971564778</v>
+        <v>0.77595188461435272</v>
       </c>
       <c r="T50">
         <v>72</v>
       </c>
       <c r="U50">
-        <v>0.81872001783841042</v>
+        <v>0.84570516614238223</v>
       </c>
       <c r="V50">
-        <v>0.18127998216158961</v>
-      </c>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.15429483385761777</v>
+      </c>
+    </row>
+    <row r="51">
       <c r="A51">
         <v>73</v>
       </c>
       <c r="B51">
-        <v>0.61910772755801813</v>
+        <v>0.84214408208228497</v>
       </c>
       <c r="C51">
-        <v>0.38089227244198182</v>
+        <v>0.15785591791771492</v>
       </c>
       <c r="H51">
         <v>73</v>
       </c>
       <c r="I51">
-        <v>0.44880597881326512</v>
+        <v>0.36986695326574676</v>
       </c>
       <c r="J51">
-        <v>0.55119402118673477</v>
+        <v>0.6301330467342533</v>
       </c>
       <c r="N51">
         <v>73</v>
       </c>
       <c r="O51">
-        <v>0.44880597881326517</v>
+        <v>0.23737714772538887</v>
       </c>
       <c r="P51">
-        <v>0.55119402118673488</v>
+        <v>0.76262285227461113</v>
       </c>
       <c r="T51">
         <v>73</v>
       </c>
       <c r="U51">
-        <v>0.82035552621929553</v>
+        <v>0.84497193883954302</v>
       </c>
       <c r="V51">
-        <v>0.1796444737807045</v>
-      </c>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.15502806116045689</v>
+      </c>
+    </row>
+    <row r="52">
       <c r="A52">
         <v>74</v>
       </c>
       <c r="B52">
-        <v>0.6268428684555073</v>
+        <v>0.82984200899908267</v>
       </c>
       <c r="C52">
-        <v>0.37315713154449259</v>
+        <v>0.17015799100091736</v>
       </c>
       <c r="H52">
         <v>74</v>
       </c>
       <c r="I52">
-        <v>0.44501977283116417</v>
+        <v>0.37699773449049984</v>
       </c>
       <c r="J52">
-        <v>0.55498022716883588</v>
+        <v>0.62300226550950011</v>
       </c>
       <c r="N52">
         <v>74</v>
       </c>
       <c r="O52">
-        <v>0.44501977283116417</v>
+        <v>0.22768528535227739</v>
       </c>
       <c r="P52">
-        <v>0.55498022716883588</v>
+        <v>0.77231471464772261</v>
       </c>
       <c r="T52">
         <v>74</v>
       </c>
       <c r="U52">
-        <v>0.84586496115780629</v>
+        <v>0.86969317298901772</v>
       </c>
       <c r="V52">
-        <v>0.15413503884219365</v>
-      </c>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+        <v>0.13030682701098231</v>
+      </c>
+    </row>
+    <row r="53">
       <c r="A53">
         <v>75</v>
       </c>
       <c r="B53">
-        <v>0.66748022878917079</v>
+        <v>0.85452926028237308</v>
       </c>
       <c r="C53">
-        <v>0.33251977121082921</v>
+        <v>0.14547073971762686</v>
       </c>
       <c r="H53">
         <v>75</v>
       </c>
       <c r="I53">
-        <v>0.45299571507755221</v>
+        <v>0.38660759586311116</v>
       </c>
       <c r="J53">
-        <v>0.54700428492244779</v>
+        <v>0.61339240413688889</v>
       </c>
       <c r="N53">
         <v>75</v>
       </c>
       <c r="O53">
-        <v>0.45299571507755221</v>
+        <v>0.42502006954003352</v>
       </c>
       <c r="P53">
-        <v>0.54700428492244779</v>
+        <v>0.57497993045996654</v>
       </c>
       <c r="T53">
         <v>75</v>
       </c>
       <c r="U53">
-        <v>0.81708916235380391</v>
+        <v>0.83576238678008974</v>
       </c>
       <c r="V53">
-        <v>0.18291083764619609</v>
+        <v>0.16423761321991023</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>